<commit_message>
add: field design excel
</commit_message>
<xml_diff>
--- a/bgf_qgis_3.x_example/bgf_lookup/BGF_typology_lookup.xlsx
+++ b/bgf_qgis_3.x_example/bgf_lookup/BGF_typology_lookup.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willeke.acampo\git\ac-willeke\BGF-QGIS\bgf_qgis_3.x_example\bgf_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B7E1D7-1494-4DEB-9DE2-F2023611C238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8E356B-8EBA-44E5-81EA-FD015014F8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="LUT_norm" sheetId="2" r:id="rId2"/>
     <sheet name="LUT_typology" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId4"/>
-    <sheet name="typology_crosswalk_no" sheetId="6" r:id="rId5"/>
-    <sheet name="LUT_weight" sheetId="4" r:id="rId6"/>
-    <sheet name="LUT_cost" sheetId="5" r:id="rId7"/>
+    <sheet name="LUT_weight" sheetId="4" r:id="rId4"/>
+    <sheet name="LUT_cost" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="215">
   <si>
     <t>BGF-QGIS-v3.x</t>
   </si>
@@ -685,15 +683,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vektingsfaktor per m2 trekroneareal, kun for SN. </t>
-  </si>
-  <si>
-    <t>BGF hovedtypologi</t>
-  </si>
-  <si>
-    <t>BGF undertypologi (Norm: PBE 2023)</t>
-  </si>
-  <si>
-    <t>BGF undertypologi (Norm: PBE 2020)</t>
   </si>
 </sst>
 </file>
@@ -1111,11 +1100,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1024" width="15"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="1024" width="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2247,552 +2239,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C947A4-11F0-4C43-AF6C-A7EB4D573D79}">
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" t="s">
-        <v>194</v>
-      </c>
-      <c r="C21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>182</v>
-      </c>
-      <c r="B22" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" t="s">
-        <v>196</v>
-      </c>
-      <c r="C23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AC71B3-77EA-42B0-A553-A3486B2558FB}">
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" t="s">
-        <v>155</v>
-      </c>
-      <c r="C18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" t="s">
-        <v>194</v>
-      </c>
-      <c r="C21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>182</v>
-      </c>
-      <c r="B22" t="s">
-        <v>195</v>
-      </c>
-      <c r="C22" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" t="s">
-        <v>196</v>
-      </c>
-      <c r="C23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A23"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3284,12 +2735,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>